<commit_message>
UST to EST, ticker_list.xlsx to predict from list.
</commit_message>
<xml_diff>
--- a/Stock_Market/user_list/user_list.xlsx
+++ b/Stock_Market/user_list/user_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Public_Github\Sentiment_Analysis\Stock_Market\user_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A995B40-2AE7-4E15-B318-60F332130A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178286AB-B724-482F-AA13-875BAA739864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12900" yWindow="-15240" windowWidth="21600" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="user_names" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>short_term</t>
   </si>
@@ -107,9 +107,6 @@
   </si>
   <si>
     <t>EconguyRosie</t>
-  </si>
-  <si>
-    <t>elonmusk</t>
   </si>
   <si>
     <t>JeffBezos</t>
@@ -537,7 +534,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -555,7 +552,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -586,9 +583,6 @@
       </c>
       <c r="B4" t="s">
         <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added Back Some Twitter Users.
</commit_message>
<xml_diff>
--- a/Stock_Market/user_list/user_list.xlsx
+++ b/Stock_Market/user_list/user_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Public_Github\Sentiment_Analysis\Stock_Market\user_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178286AB-B724-482F-AA13-875BAA739864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B62C896-E6C7-4F0A-98D2-788BF0F71214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1548" yWindow="1176" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="user_names" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>short_term</t>
   </si>
@@ -116,6 +116,15 @@
   </si>
   <si>
     <t>controversial</t>
+  </si>
+  <si>
+    <t>AswathDamodaran</t>
+  </si>
+  <si>
+    <t>cstewartcfa</t>
+  </si>
+  <si>
+    <t>BobPisani</t>
   </si>
 </sst>
 </file>
@@ -534,13 +543,13 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.88671875" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -629,15 +638,24 @@
       <c r="A10" t="s">
         <v>10</v>
       </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>